<commit_message>
Fixed setlist import bug - missing </Song> terminator.
</commit_message>
<xml_diff>
--- a/0300_MetadataTransformSpreadheet.xlsx
+++ b/0300_MetadataTransformSpreadheet.xlsx
@@ -390,7 +390,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -632,7 +632,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="580" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -726,7 +726,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -773,37 +773,37 @@
       </c>
     </row>
     <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!A2</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!B2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!E2</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!F2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!G2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!H2</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="13" t="n">
-        <f aca="false">'forScore CSV Export'!I2</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="13" t="n">
-        <f aca="false">IntermediateCalcs!I2</f>
-        <v>0</v>
+      <c r="A2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!A2),"",'forScore CSV Export'!A2)</f>
+        <v/>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!B2),"",'forScore CSV Export'!B2)</f>
+        <v/>
+      </c>
+      <c r="C2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!E2),"",'forScore CSV Export'!E2)</f>
+        <v/>
+      </c>
+      <c r="D2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!F2),"",'forScore CSV Export'!F2)</f>
+        <v/>
+      </c>
+      <c r="E2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!G2),"",'forScore CSV Export'!G2)</f>
+        <v/>
+      </c>
+      <c r="F2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!H2),"",'forScore CSV Export'!H2)</f>
+        <v/>
+      </c>
+      <c r="G2" s="13" t="str">
+        <f aca="false">IF(ISBLANK('forScore CSV Export'!I2),"",'forScore CSV Export'!I2)</f>
+        <v/>
+      </c>
+      <c r="H2" s="13" t="str">
+        <f aca="false">IF(IntermediateCalcs!I2&lt;=0,"",IntermediateCalcs!I2)</f>
+        <v/>
       </c>
       <c r="I2" s="14" t="str">
         <f aca="false">IntermediateCalcs!H2</f>

</xml_diff>